<commit_message>
Gen3 changed to Synchronous Condenser
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee9/ieee9_2025.xlsx
+++ b/data/IEEE9/ieee9/ieee9_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7760944B-5C19-4780-972F-1EC6A2FBA1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5A6CBC-5B98-4230-80C2-561212ADCC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="3255" windowWidth="21600" windowHeight="12660" tabRatio="722" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7365" yWindow="3765" windowWidth="21600" windowHeight="12660" tabRatio="722" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13088,8 +13088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42CD27A-91A8-4D31-B70E-255219E25912}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13253,76 +13253,76 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -13330,76 +13330,76 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27071,8 +27071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6451C0BC-1134-43AA-AB38-9EE91B1398E3}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27236,76 +27236,76 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -27313,76 +27313,76 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>